<commit_message>
MOM Week 2 Data Added
</commit_message>
<xml_diff>
--- a/MOM2024/week2.xlsx
+++ b/MOM2024/week2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffpch\Desktop\Tableau\MM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivektiwari/Code/Programming/Tableau/MOM2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCD5233-99B9-404F-AA0B-70FFB5EBF7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C63C154-8644-5F4B-AC4E-3CF970FEC263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{08ADAA6D-1873-42BA-8833-7C5ADDE25218}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{08ADAA6D-1873-42BA-8833-7C5ADDE25218}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 50" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Top 50'!$A$1:$F$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,9 +44,6 @@
     <t>Cristiano Ronaldo</t>
   </si>
   <si>
-    <t>Soccer</t>
-  </si>
-  <si>
     <t>Lionel Messi</t>
   </si>
   <si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Off-the-Field Earnings</t>
+  </si>
+  <si>
+    <t>American Football</t>
   </si>
 </sst>
 </file>
@@ -235,8 +238,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -273,17 +276,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -602,40 +605,40 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -643,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2">
         <v>136000000</v>
@@ -655,15 +658,15 @@
         <v>90000000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2">
         <v>130000000</v>
@@ -675,15 +678,15 @@
         <v>65000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>120000000</v>
@@ -695,15 +698,15 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="2">
         <v>119500000</v>
@@ -715,15 +718,15 @@
         <v>75000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>110000000</v>
@@ -735,15 +738,15 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>107000000</v>
@@ -755,15 +758,15 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>106000000</v>
@@ -775,15 +778,15 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2">
         <v>100400000</v>
@@ -795,15 +798,15 @@
         <v>52000000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D10" s="2">
         <v>95100000</v>
@@ -815,15 +818,15 @@
         <v>95000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2">
         <v>89100000</v>
@@ -835,15 +838,15 @@
         <v>45000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2">
         <v>87600000</v>
@@ -855,15 +858,15 @@
         <v>45000000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>85000000</v>
@@ -875,15 +878,15 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2">
         <v>85000000</v>
@@ -895,15 +898,15 @@
         <v>13000000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2">
         <v>82100000</v>
@@ -915,15 +918,15 @@
         <v>35000000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2">
         <v>80800000</v>
@@ -935,15 +938,15 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2">
         <v>75100000</v>
@@ -955,15 +958,15 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2">
         <v>73000000</v>
@@ -975,15 +978,15 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="2">
         <v>72000000</v>
@@ -995,15 +998,15 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2">
         <v>70500000</v>
@@ -1015,15 +1018,15 @@
         <v>3500000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="2">
         <v>69000000</v>
@@ -1035,15 +1038,15 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D22" s="2">
         <v>65000000</v>
@@ -1055,15 +1058,15 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2">
         <v>64000000</v>
@@ -1075,15 +1078,15 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2">
         <v>60900000</v>
@@ -1095,15 +1098,15 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2">
         <v>59300000</v>
@@ -1115,15 +1118,15 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2">
         <v>58600000</v>
@@ -1135,15 +1138,15 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D27" s="2">
         <v>56700000</v>
@@ -1155,15 +1158,15 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2">
         <v>55100000</v>
@@ -1175,15 +1178,15 @@
         <v>22000000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2">
         <v>53000000</v>
@@ -1195,15 +1198,15 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" s="2">
         <v>53000000</v>
@@ -1215,15 +1218,15 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2">
         <v>53000000</v>
@@ -1235,15 +1238,15 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2">
         <v>53000000</v>
@@ -1255,15 +1258,15 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D33" s="2">
         <v>52000000</v>
@@ -1275,15 +1278,15 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="2">
         <v>52000000</v>
@@ -1295,15 +1298,15 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2">
         <v>51500000</v>
@@ -1315,15 +1318,15 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2">
         <v>50500000</v>
@@ -1335,15 +1338,15 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="2">
         <v>49800000</v>
@@ -1355,15 +1358,15 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2">
         <v>48900000</v>
@@ -1375,15 +1378,15 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D39" s="2">
         <v>48600000</v>
@@ -1395,15 +1398,15 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D40" s="2">
         <v>48500000</v>
@@ -1415,15 +1418,15 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D41" s="2">
         <v>48000000</v>
@@ -1435,15 +1438,15 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2">
         <v>47800000</v>
@@ -1455,15 +1458,15 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43" s="2">
         <v>47800000</v>
@@ -1475,15 +1478,15 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" s="2">
         <v>47500000</v>
@@ -1495,15 +1498,15 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D45" s="2">
         <v>47200000</v>
@@ -1515,15 +1518,15 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" s="2">
         <v>47100000</v>
@@ -1535,15 +1538,15 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2">
         <v>46000000</v>
@@ -1555,15 +1558,15 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D48" s="2">
         <v>46000000</v>
@@ -1575,15 +1578,15 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D49" s="2">
         <v>45800000</v>
@@ -1595,15 +1598,15 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="2">
         <v>45300000</v>
@@ -1615,15 +1618,15 @@
         <v>45000000</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D51" s="2">
         <v>45200000</v>

</xml_diff>